<commit_message>
added graphs to metrics excel
</commit_message>
<xml_diff>
--- a/doc/Metrics.xlsx
+++ b/doc/Metrics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
   <si>
     <t>Metrics Tracking</t>
   </si>
@@ -74,6 +74,12 @@
   <si>
     <t>Notes</t>
   </si>
+  <si>
+    <t>Nested Depth</t>
+  </si>
+  <si>
+    <t>Cyclomatic Complexity</t>
+  </si>
 </sst>
 </file>
 
@@ -113,10 +119,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,6 +135,1049 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Method Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$33:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.1293333333333324</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6639999999999988</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5419999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3235000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.3005000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.2097500000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9882499999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.7075000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.7489999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="34296576"/>
+        <c:axId val="34298112"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="34296576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="34298112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="34298112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="34296576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>D.O.I. Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$33:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.5986666666666665</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4880000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3660000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8772499999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8772499999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8772499999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6772499999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.452</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.48075</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="32032640"/>
+        <c:axId val="32034176"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="32032640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="32034176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="32034176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="32032640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nested Depth</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$33:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.155</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.258</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.39375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4340000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4340000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4064999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3645</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.355</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="34651520"/>
+        <c:axId val="34653312"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="34651520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="34653312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="34653312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="34651520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cyclomatic Complexity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$33:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.8949999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.015333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2610000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1890000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1252500000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1252500000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1080000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9584999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9889999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="35330304"/>
+        <c:axId val="35336192"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="35330304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="35336192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="35336192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="35330304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Afferent Coupling</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$33:$G$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.83333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="75043200"/>
+        <c:axId val="75044736"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="75043200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75044736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="75044736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75043200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LOC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$33:$H$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>919</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1279</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1578</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1689</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1678</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1713</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="82272256"/>
+        <c:axId val="82273792"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="82272256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82273792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="82273792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82272256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1264920</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,45 +1491,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -520,13 +1569,13 @@
       <c r="O3" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="2"/>
+      <c r="R3" s="3"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>41025</v>
       </c>
       <c r="C4">
@@ -573,7 +1622,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>41026</v>
       </c>
       <c r="C5">
@@ -620,7 +1669,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>41030</v>
       </c>
       <c r="C6">
@@ -667,7 +1716,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>41032</v>
       </c>
       <c r="C7">
@@ -714,7 +1763,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>41036</v>
       </c>
       <c r="C8">
@@ -761,7 +1810,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>41037</v>
       </c>
       <c r="C9">
@@ -808,7 +1857,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>41038</v>
       </c>
       <c r="C10">
@@ -849,7 +1898,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>41039</v>
       </c>
       <c r="C11">
@@ -890,7 +1939,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>41040</v>
       </c>
       <c r="C12">
@@ -931,33 +1980,33 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>41042</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+      <c r="A15" s="2"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="J17" s="2" t="s">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="J17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
@@ -998,7 +2047,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>41025</v>
       </c>
       <c r="C19">
@@ -1039,7 +2088,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>41026</v>
       </c>
       <c r="C20">
@@ -1080,7 +2129,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>41030</v>
       </c>
       <c r="C21">
@@ -1121,7 +2170,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>41032</v>
       </c>
       <c r="C22">
@@ -1162,7 +2211,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>41036</v>
       </c>
       <c r="C23">
@@ -1203,7 +2252,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>41037</v>
       </c>
       <c r="C24">
@@ -1244,7 +2293,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>41038</v>
       </c>
       <c r="C25">
@@ -1285,7 +2334,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>41039</v>
       </c>
       <c r="C26">
@@ -1326,7 +2375,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>41040</v>
       </c>
       <c r="C27">
@@ -1367,22 +2416,22 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>41042</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
+      <c r="A29" s="2"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
@@ -1392,10 +2441,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G32" t="s">
         <v>9</v>
@@ -1405,27 +2454,27 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="3">
+      <c r="A33" s="2">
         <v>41025</v>
       </c>
       <c r="C33">
-        <f>(C4+J4+J19)/3</f>
+        <f t="shared" ref="C33:G34" si="0">(C4+J4+J19)/3</f>
         <v>4.1293333333333324</v>
       </c>
       <c r="D33">
-        <f>(D4+K4+K19)/3</f>
+        <f t="shared" si="0"/>
         <v>1.5986666666666665</v>
       </c>
       <c r="E33">
-        <f>(E4+L4+L19)/3</f>
+        <f t="shared" si="0"/>
         <v>1.155</v>
       </c>
       <c r="F33">
-        <f>(F4+M4+M19)/3</f>
+        <f t="shared" si="0"/>
         <v>1.8949999999999998</v>
       </c>
       <c r="G33">
-        <f>(G4+N4+N19)/3</f>
+        <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="H33">
@@ -1434,27 +2483,27 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
+      <c r="A34" s="2">
         <v>41026</v>
       </c>
       <c r="C34">
-        <f>(C5+J5+J20)/3</f>
+        <f t="shared" si="0"/>
         <v>5.6639999999999988</v>
       </c>
       <c r="D34">
-        <f>(D5+K5+K20)/3</f>
+        <f t="shared" si="0"/>
         <v>1.4880000000000002</v>
       </c>
       <c r="E34">
-        <f>(E5+L5+L20)/3</f>
+        <f t="shared" si="0"/>
         <v>1.258</v>
       </c>
       <c r="F34">
-        <f>(F5+M5+M20)/3</f>
+        <f t="shared" si="0"/>
         <v>2.015333333333333</v>
       </c>
       <c r="G34">
-        <f>(G5+N5+N20)/3</f>
+        <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="H34">
@@ -1463,210 +2512,210 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="3">
+      <c r="A35" s="2">
         <v>41030</v>
       </c>
       <c r="C35">
-        <f>SUM(C6,J6,C21,J21) / 4</f>
+        <f t="shared" ref="C35:G41" si="1">SUM(C6,J6,C21,J21) / 4</f>
         <v>6.5419999999999998</v>
       </c>
       <c r="D35">
-        <f>SUM(D6,K6,D21,K21) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.3660000000000001</v>
       </c>
       <c r="E35">
-        <f>SUM(E6,L6,E21,L21) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.333</v>
       </c>
       <c r="F35">
-        <f>SUM(F6,M6,F21,M21) / 4</f>
+        <f t="shared" si="1"/>
         <v>2.2610000000000001</v>
       </c>
       <c r="G35">
-        <f>SUM(G6,N6,G21,N21) / 4</f>
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
       <c r="H35">
-        <f>SUM(H6,O6,H21,O21)</f>
+        <f t="shared" ref="H35:H41" si="2">SUM(H6,O6,H21,O21)</f>
         <v>1279</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="3">
+      <c r="A36" s="2">
         <v>41032</v>
       </c>
       <c r="C36">
-        <f>SUM(C7,J7,C22,J22) / 4</f>
+        <f t="shared" si="1"/>
         <v>7.3235000000000001</v>
       </c>
       <c r="D36">
-        <f>SUM(D7,K7,D22,K22) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.8772499999999999</v>
       </c>
       <c r="E36">
-        <f>SUM(E7,L7,E22,L22) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.39375</v>
       </c>
       <c r="F36">
-        <f>SUM(F7,M7,F22,M22) / 4</f>
+        <f t="shared" si="1"/>
         <v>2.1890000000000001</v>
       </c>
       <c r="G36">
-        <f>SUM(G7,N7,G22,N22) / 4</f>
+        <f t="shared" si="1"/>
         <v>2.125</v>
       </c>
       <c r="H36">
-        <f>SUM(H7,O7,H22,O22)</f>
+        <f t="shared" si="2"/>
         <v>1578</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="3">
+      <c r="A37" s="2">
         <v>41036</v>
       </c>
       <c r="C37">
-        <f>SUM(C8,J8,C23,J23) / 4</f>
+        <f t="shared" si="1"/>
         <v>7.3005000000000004</v>
       </c>
       <c r="D37">
-        <f>SUM(D8,K8,D23,K23) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.8772499999999999</v>
       </c>
       <c r="E37">
-        <f>SUM(E8,L8,E23,L23) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.4340000000000002</v>
       </c>
       <c r="F37">
-        <f>SUM(F8,M8,F23,M23) / 4</f>
+        <f t="shared" si="1"/>
         <v>2.1252500000000003</v>
       </c>
       <c r="G37">
-        <f>SUM(G8,N8,G23,N23) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="H37">
-        <f>SUM(H8,O8,H23,O23)</f>
+        <f t="shared" si="2"/>
         <v>1689</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="3">
+      <c r="A38" s="2">
         <v>41037</v>
       </c>
       <c r="C38">
-        <f>SUM(C9,J9,C24,J24) / 4</f>
+        <f t="shared" si="1"/>
         <v>7.2097500000000005</v>
       </c>
       <c r="D38">
-        <f>SUM(D9,K9,D24,K24) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.8772499999999999</v>
       </c>
       <c r="E38">
-        <f>SUM(E9,L9,E24,L24) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.4340000000000002</v>
       </c>
       <c r="F38">
-        <f>SUM(F9,M9,F24,M24) / 4</f>
+        <f t="shared" si="1"/>
         <v>2.1252500000000003</v>
       </c>
       <c r="G38">
-        <f>SUM(G9,N9,G24,N24) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="H38">
-        <f>SUM(H9,O9,H24,O24)</f>
+        <f t="shared" si="2"/>
         <v>1678</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="3">
+      <c r="A39" s="2">
         <v>41038</v>
       </c>
       <c r="C39">
-        <f>SUM(C10,J10,C25,J25) / 4</f>
+        <f t="shared" si="1"/>
         <v>6.9882499999999999</v>
       </c>
       <c r="D39">
-        <f>SUM(D10,K10,D25,K25) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.6772499999999999</v>
       </c>
       <c r="E39">
-        <f>SUM(E10,L10,E25,L25) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.4064999999999999</v>
       </c>
       <c r="F39">
-        <f>SUM(F10,M10,F25,M25) / 4</f>
+        <f t="shared" si="1"/>
         <v>2.1080000000000001</v>
       </c>
       <c r="G39">
-        <f>SUM(G10,N10,G25,N25) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="H39">
-        <f>SUM(H10,O10,H25,O25)</f>
+        <f t="shared" si="2"/>
         <v>1713</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="3">
+      <c r="A40" s="2">
         <v>41039</v>
       </c>
       <c r="C40">
-        <f>SUM(C11,J11,C26,J26) / 4</f>
+        <f t="shared" si="1"/>
         <v>6.7075000000000005</v>
       </c>
       <c r="D40">
-        <f>SUM(D11,K11,D26,K26) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.452</v>
       </c>
       <c r="E40">
-        <f>SUM(E11,L11,E26,L26) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.3645</v>
       </c>
       <c r="F40">
-        <f>SUM(F11,M11,F26,M26) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.9584999999999999</v>
       </c>
       <c r="G40">
-        <f>SUM(G11,N11,G26,N26) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
       <c r="H40">
-        <f>SUM(H11,O11,H26,O26)</f>
+        <f t="shared" si="2"/>
         <v>1977</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="3">
+      <c r="A41" s="2">
         <v>41040</v>
       </c>
       <c r="C41">
-        <f>SUM(C12,J12,C27,J27) / 4</f>
+        <f t="shared" si="1"/>
         <v>6.7489999999999997</v>
       </c>
       <c r="D41">
-        <f>SUM(D12,K12,D27,K27) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.48075</v>
       </c>
       <c r="E41">
-        <f>SUM(E12,L12,E27,L27) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.355</v>
       </c>
       <c r="F41">
-        <f>SUM(F12,M12,F27,M27) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.9889999999999999</v>
       </c>
       <c r="G41">
-        <f>SUM(G12,N12,G27,N27) / 4</f>
+        <f t="shared" si="1"/>
         <v>1.6875</v>
       </c>
       <c r="H41">
-        <f>SUM(H12,O12,H27,O27)</f>
+        <f t="shared" si="2"/>
         <v>2140</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="3">
+      <c r="A42" s="2">
         <v>41042</v>
       </c>
     </row>
@@ -1681,6 +2730,7 @@
     <mergeCell ref="J17:O17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>